<commit_message>
- loading added - response handling - data response stability
</commit_message>
<xml_diff>
--- a/serverEmulation/cdn/financeCalculator.xlsx
+++ b/serverEmulation/cdn/financeCalculator.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="price1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="135">
   <si>
     <t>option1</t>
   </si>
@@ -426,31 +426,16 @@
     <t>16 200</t>
   </si>
   <si>
-    <t>от 101 и выше</t>
-  </si>
-  <si>
-    <t>230 
-руб/шт</t>
-  </si>
-  <si>
-    <t>216  
-руб/шт</t>
-  </si>
-  <si>
-    <t>243  
-руб/шт</t>
-  </si>
-  <si>
-    <t>270 
-руб/шт</t>
-  </si>
-  <si>
-    <t>135  
-руб/шт</t>
-  </si>
-  <si>
-    <t>162  
-руб/шт</t>
+    <r>
+      <t xml:space="preserve">от 101 и выше
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>руб/шт</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1454,26 +1439,26 @@
       <c r="B23" s="5">
         <v>1.0</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>139</v>
+      <c r="C23" s="10">
+        <v>230.0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>216.0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>243.0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>270.0</v>
+      </c>
+      <c r="G23" s="12">
+        <v>135.0</v>
+      </c>
+      <c r="H23" s="12">
+        <v>162.0</v>
+      </c>
+      <c r="I23" s="12">
+        <v>135.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>